<commit_message>
feat: add user profile and personal information pages with detailed employee data display.
</commit_message>
<xml_diff>
--- a/شجرة الارتباطات.xlsx
+++ b/شجرة الارتباطات.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhan\OneDrive\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhanad\Desktop\Projects\MDOC HRMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64047602-AE62-4511-8F3E-2DE29B5A92A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA02B951-5562-4D19-90AD-D6BF3D56D2BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -229,12 +229,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -264,13 +270,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -554,35 +563,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="16.44140625" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -593,7 +605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -604,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -615,7 +627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -626,7 +638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -637,7 +649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -648,7 +660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -659,7 +671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -670,7 +682,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -681,7 +693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -692,7 +704,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -703,7 +715,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -714,7 +726,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -725,7 +737,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -736,7 +748,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -747,7 +759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -758,7 +770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -769,7 +781,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
@@ -780,7 +792,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>35</v>
       </c>
@@ -791,7 +803,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -802,7 +814,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
@@ -813,7 +825,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
@@ -824,7 +836,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
@@ -835,7 +847,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
@@ -846,7 +858,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -857,7 +869,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
@@ -868,7 +880,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -879,7 +891,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -890,7 +902,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -901,7 +913,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -912,7 +924,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>43</v>
       </c>
@@ -923,7 +935,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>44</v>
       </c>
@@ -934,7 +946,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -945,7 +957,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>45</v>
       </c>
@@ -956,7 +968,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
@@ -967,7 +979,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
@@ -978,7 +990,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>48</v>
       </c>
@@ -989,7 +1001,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>49</v>
       </c>
@@ -1000,7 +1012,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>50</v>
       </c>
@@ -1011,7 +1023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>51</v>
       </c>
@@ -1022,7 +1034,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>52</v>
       </c>
@@ -1033,7 +1045,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>53</v>
       </c>
@@ -1044,7 +1056,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>54</v>
       </c>
@@ -1055,7 +1067,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>55</v>
       </c>
@@ -1066,7 +1078,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>28</v>
       </c>
@@ -1077,7 +1089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
@@ -1088,7 +1100,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>56</v>
       </c>
@@ -1099,7 +1111,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>57</v>
       </c>
@@ -1110,7 +1122,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>58</v>
       </c>
@@ -1121,7 +1133,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>59</v>
       </c>
@@ -1132,7 +1144,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>60</v>
       </c>

</xml_diff>